<commit_message>
update '#12 Merge cell, data validation (BKIndex Group).xlsx'
</commit_message>
<xml_diff>
--- a/contents/Tuan1/Video6/#12 Merge cell, data validation (BKIndex Group).xlsx
+++ b/contents/Tuan1/Video6/#12 Merge cell, data validation (BKIndex Group).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvn20206205\Desktop\20232\Datawarehouse\contents\Tuan1\Video6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7AEA35-42B4-49AE-BD77-55529F3353A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PI-O'LE" sheetId="1" r:id="rId1"/>
@@ -13,13 +19,27 @@
     <sheet name="WorkSpace2" sheetId="4" r:id="rId4"/>
     <sheet name="Sumup" sheetId="5" r:id="rId5"/>
     <sheet name="QA&amp;Practice" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="DS_DO_AN">WorkSpace2!$M$7:$M$9</definedName>
     <definedName name="DS_DO_UONG">WorkSpace2!$N$7:$N$9</definedName>
     <definedName name="test">WorkSpace2!$K$12:$K$14</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -228,7 +248,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -549,7 +569,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -571,7 +591,6 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -584,12 +603,9 @@
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -623,13 +639,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma 9" xfId="4"/>
+    <cellStyle name="Comma 9" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_DE_15 8" xfId="3"/>
+    <cellStyle name="Normal_DE_15 8" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -638,6 +657,14 @@
       <color rgb="FF0000CC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -660,6 +687,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1" descr="Piole v1.0.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -705,6 +737,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4" descr="logo BKIndex.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -743,7 +780,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="324640_10151130207401897_27487587_o.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="324640_10151130207401897_27487587_o.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -781,7 +824,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Down Arrow 3"/>
+        <xdr:cNvPr id="4" name="Down Arrow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -840,20 +889,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1"/>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6950213" cy="647701"/>
+          <a:ext cx="7014983" cy="624841"/>
           <a:chOff x="5810251" y="49917"/>
           <a:chExt cx="5817062" cy="629265"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2"/>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -907,7 +968,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Right Triangle 3"/>
+          <xdr:cNvPr id="4" name="Right Triangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -961,7 +1028,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4"/>
+          <xdr:cNvPr id="5" name="Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1025,7 +1098,7 @@
               <a:t> 12:  </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="0" baseline="0" smtClean="0">
+              <a:rPr lang="en-US" sz="1600" b="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="bg1"/>
                 </a:solidFill>
@@ -1062,6 +1135,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="Picture 5" descr="logo BKIndex.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1105,20 +1183,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1"/>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8826638" cy="647701"/>
+          <a:ext cx="8996183" cy="624841"/>
           <a:chOff x="5810251" y="49917"/>
           <a:chExt cx="5817062" cy="629265"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2"/>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1172,7 +1262,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Right Triangle 3"/>
+          <xdr:cNvPr id="4" name="Right Triangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1226,7 +1322,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4"/>
+          <xdr:cNvPr id="5" name="Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1290,7 +1392,7 @@
               <a:t> 12:  </a:t>
             </a:r>
             <a:r>
-              <a:rPr kumimoji="0" lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+              <a:rPr kumimoji="0" lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -1330,6 +1432,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="Picture 5" descr="logo BKIndex.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1375,6 +1482,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1" descr="logo BKIndex.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1418,20 +1530,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="Group 2"/>
+        <xdr:cNvPr id="3" name="Group 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8172450" cy="647701"/>
+          <a:ext cx="8199120" cy="624841"/>
           <a:chOff x="5810251" y="49917"/>
           <a:chExt cx="5817062" cy="629265"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3"/>
+          <xdr:cNvPr id="4" name="Rectangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1507,7 +1631,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Right Triangle 4"/>
+          <xdr:cNvPr id="5" name="Right Triangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1561,7 +1691,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle 5"/>
+          <xdr:cNvPr id="6" name="Rectangle 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1634,7 +1770,7 @@
               <a:t>Bài 12:  </a:t>
             </a:r>
             <a:r>
-              <a:rPr kumimoji="0" lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+              <a:rPr kumimoji="0" lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -1650,20 +1786,6 @@
               </a:rPr>
               <a:t>Merge cell, Data Validation</a:t>
             </a:r>
-            <a:endParaRPr kumimoji="0" lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:prstClr val="white"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1687,6 +1809,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="Picture 6" descr="logo BKIndex.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1714,9 +1841,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1754,7 +1881,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1788,6 +1915,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1822,9 +1950,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1997,7 +2126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2007,9 +2136,9 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="12" max="12" width="84.5703125" customWidth="1"/>
+    <col min="12" max="12" width="84.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="12:12">
@@ -2022,7 +2151,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="12:12" ht="30">
+    <row r="22" spans="12:12" ht="28.8">
       <c r="L22" s="12" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2159,7 @@
   </sheetData>
   <sheetProtection password="C5FD" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2039,32 +2168,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="155.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="155.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="100.5" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:2" ht="100.5" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-    </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="18.75">
+    </row>
+    <row r="2" spans="1:2" s="4" customFormat="1" ht="18">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2072,33 +2200,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="33"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="34"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="21" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="31"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="32"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="19.5">
+    <row r="24" spans="2:2" ht="19.8">
       <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
@@ -2111,7 +2239,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="B2" location="Casestudy!A29" display="Đáp án"/>
+    <hyperlink ref="B2" location="Casestudy!A29" display="Đáp án" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2120,7 +2248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0000CC"/>
   </sheetPr>
@@ -2130,11 +2258,11 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:9" ht="21" customHeight="1">
@@ -2151,10 +2279,10 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2164,10 +2292,10 @@
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="19" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2177,48 +2305,48 @@
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="36" t="str">
+      <c r="H8" s="34" t="str">
         <f t="shared" ref="H8:H9" si="0">H7</f>
         <v>Toán Tin 1</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="H9" s="36" t="str">
+      <c r="H9" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Toán Tin 1</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1">
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1">
-      <c r="H11" s="35" t="str">
+      <c r="H11" s="33" t="str">
         <f t="shared" ref="H11:H12" si="1">H10</f>
         <v>Toán Tin 2</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21" customHeight="1">
-      <c r="H12" s="35" t="str">
+      <c r="H12" s="33" t="str">
         <f t="shared" si="1"/>
         <v>Toán Tin 2</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2297,27 +2425,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0000CC"/>
   </sheetPr>
   <dimension ref="A6:N34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" customWidth="1"/>
+    <col min="11" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:14" ht="21" customHeight="1">
@@ -2328,14 +2456,14 @@
         <v>22</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="27" t="s">
+      <c r="L6" s="24"/>
+      <c r="M6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="28" t="s">
+      <c r="N6" s="26" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2345,25 +2473,25 @@
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="24" t="s">
+      <c r="M7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2373,25 +2501,25 @@
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="24" t="s">
+      <c r="M8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2401,11 +2529,11 @@
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="M9" s="24" t="s">
+      <c r="G9" s="15"/>
+      <c r="M9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2415,32 +2543,32 @@
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:14" ht="21" customHeight="1">
       <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75">
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.6">
       <c r="C12" s="2"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.75">
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:14" ht="15.75">
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75">
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75">
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="7:10" ht="15.75">
-      <c r="G17" s="17"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.6">
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.6">
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.6">
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.6">
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="7:10" ht="15.6">
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="7:10">
       <c r="G18" s="10"/>
@@ -2496,7 +2624,7 @@
     <protectedRange sqref="G6:G17" name="Bảng lương"/>
   </protectedRanges>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>INDIRECT(DS_DO_AN)</formula1>
     </dataValidation>
   </dataValidations>
@@ -2507,7 +2635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -2517,12 +2645,12 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="39">
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="38.4">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -2626,7 +2754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -2636,22 +2764,22 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:2" ht="27" customHeight="1">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="40.5" customHeight="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="18"/>
     </row>
   </sheetData>
   <sheetProtection password="C5FD" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
@@ -2661,4 +2789,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96F8B49-31D3-46BA-BA11-72F0F9EC6BCA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update Tuan1.md, Tuan1.tex and '#12 Merge cell, data validation (BKIndex Group).xlsx'
</commit_message>
<xml_diff>
--- a/contents/Tuan1/Video6/#12 Merge cell, data validation (BKIndex Group).xlsx
+++ b/contents/Tuan1/Video6/#12 Merge cell, data validation (BKIndex Group).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvn20206205\Desktop\20232\Datawarehouse\contents\Tuan1\Video6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvn20206205\Desktop\Datawarehouse\contents\Tuan1\Video6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7AEA35-42B4-49AE-BD77-55529F3353A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E3D3B3-3C23-4164-BFBE-D6B75B31549E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2432,7 +2432,7 @@
   <dimension ref="A6:N34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2505,7 +2505,7 @@
         <v>42</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>33</v>
@@ -2544,6 +2544,9 @@
         <v>26</v>
       </c>
       <c r="G10" s="15"/>
+      <c r="H10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="21" customHeight="1">
       <c r="C11" s="2" t="s">
@@ -2623,9 +2626,18 @@
   <protectedRanges>
     <protectedRange sqref="G6:G17" name="Bảng lương"/>
   </protectedRanges>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>INDIRECT(DS_DO_AN)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8" xr:uid="{7E02FA0B-2056-41CA-AF12-DB84EC03BBC4}">
+      <formula1>$K$7:$K$8</formula1>
+    </dataValidation>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Bạn phải nhập số lớn hơn 0" promptTitle="Gợi ý" prompt="Phải nhập số lớn hơn 0" sqref="H10" xr:uid="{7CE2C7EA-F070-442F-8173-875D386D6BC2}">
+      <formula1>H10&gt;0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20" xr:uid="{0752A4C0-85F4-4503-B3E7-1C2AFFBA4696}">
+      <formula1>INDIRECT(VLOOKUP($H$8,$K$7:$L$8,2,FALSE))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2 files and delete 5 files
</commit_message>
<xml_diff>
--- a/contents/Tuan1/Video6/#12 Merge cell, data validation (BKIndex Group).xlsx
+++ b/contents/Tuan1/Video6/#12 Merge cell, data validation (BKIndex Group).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvn20206205\Desktop\Datawarehouse\contents\Tuan1\Video6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E3D3B3-3C23-4164-BFBE-D6B75B31549E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B443D41-FDD2-4BE1-A820-483279F05B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2432,7 +2432,7 @@
   <dimension ref="A6:N34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2508,7 +2508,7 @@
         <v>30</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>30</v>
@@ -2636,7 +2636,7 @@
     <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Bạn phải nhập số lớn hơn 0" promptTitle="Gợi ý" prompt="Phải nhập số lớn hơn 0" sqref="H10" xr:uid="{7CE2C7EA-F070-442F-8173-875D386D6BC2}">
       <formula1>H10&gt;0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20" xr:uid="{0752A4C0-85F4-4503-B3E7-1C2AFFBA4696}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20 J14 I8" xr:uid="{0752A4C0-85F4-4503-B3E7-1C2AFFBA4696}">
       <formula1>INDIRECT(VLOOKUP($H$8,$K$7:$L$8,2,FALSE))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>